<commit_message>
feat: Add generating random _id for members
</commit_message>
<xml_diff>
--- a/public/sample.xlsx
+++ b/public/sample.xlsx
@@ -11,10 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>순서</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>회원명</t>
   </si>
@@ -38,7 +35,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -55,6 +52,10 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <color rgb="FFB7B7B7"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -70,7 +71,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -79,6 +80,12 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -306,13 +313,10 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2">
-        <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
@@ -320,9 +324,36 @@
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
-      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="3"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="3"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="3"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="3"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="3"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>